<commit_message>
Renaming output_opt_detail and output_opt_detail_agg output tables to output_opt_detail_daily and output_opt_detail_weekly
</commit_message>
<xml_diff>
--- a/mro_documentation/mro_or_data_model.xlsx
+++ b/mro_documentation/mro_or_data_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\casuser\Cleveland_Clinic\gitbackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\casuser\Cleveland_Clinic\gitrepo\mro_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AB8CC6-D584-420E-B7E4-4F127A7473DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C35148-3EF2-43B1-A2E7-FAC55ACD2533}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS FOR OPTIMIZATION" sheetId="1" r:id="rId1"/>
@@ -333,9 +333,6 @@
     <t>Vascular Services</t>
   </si>
   <si>
-    <t>OUTPUT_OPT_DETAIL</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of new patients admitted without the COVID-19 testing requirements </t>
-  </si>
-  <si>
-    <t>OUTPUT_OPT_DETAIL_AGG</t>
   </si>
   <si>
     <t>DailyDemand</t>
@@ -770,6 +764,12 @@
   </si>
   <si>
     <t>Facilty2</t>
+  </si>
+  <si>
+    <t>OUTPUT_OPT_DETAIL_DAILY</t>
+  </si>
+  <si>
+    <t>OUTPUT_OPT_DETAIL_WEEKLY</t>
   </si>
 </sst>
 </file>
@@ -1305,6 +1305,21 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1318,21 +1333,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1652,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1675,29 +1675,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="F2" s="89" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="F2" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="D6" s="8"/>
       <c r="F6" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="F7" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="F8" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>18</v>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="D9" s="8"/>
       <c r="F9" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>18</v>
@@ -1967,12 +1967,12 @@
       <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
       <c r="M16" s="21"/>
       <c r="N16" s="27"/>
     </row>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="D18" s="8"/>
       <c r="F18" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>39</v>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="D19" s="8"/>
       <c r="F19" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>39</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="F20" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>42</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="F21" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>42</v>
@@ -2145,12 +2145,12 @@
       <c r="N23" s="27"/>
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
       <c r="M24" s="21"/>
       <c r="N24" s="27"/>
     </row>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="D26" s="9"/>
       <c r="F26" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>18</v>
@@ -2215,10 +2215,10 @@
       <c r="J26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="92">
+      <c r="K26" s="87">
         <v>10000</v>
       </c>
-      <c r="L26" s="92">
+      <c r="L26" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D27" s="7"/>
       <c r="F27" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>18</v>
@@ -2248,10 +2248,10 @@
       <c r="J27" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="92">
+      <c r="K27" s="87">
         <v>10000</v>
       </c>
-      <c r="L27" s="92">
+      <c r="L27" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="F28" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>18</v>
@@ -2281,10 +2281,10 @@
       <c r="J28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="92">
+      <c r="K28" s="87">
         <v>10000</v>
       </c>
-      <c r="L28" s="92">
+      <c r="L28" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="D29" s="7"/>
       <c r="F29" s="32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>18</v>
@@ -2314,10 +2314,10 @@
       <c r="J29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K29" s="92">
+      <c r="K29" s="87">
         <v>10000</v>
       </c>
-      <c r="L29" s="92">
+      <c r="L29" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="F30" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>18</v>
@@ -2347,10 +2347,10 @@
       <c r="J30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="92">
+      <c r="K30" s="87">
         <v>10000</v>
       </c>
-      <c r="L30" s="92">
+      <c r="L30" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2383,12 +2383,12 @@
       <c r="F33"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="88"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D36" s="9"/>
       <c r="F36" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>42</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="F37" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>42</v>
@@ -2699,14 +2699,14 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="87" t="s">
+      <c r="A49" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="88"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
       <c r="F49" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>42</v>
@@ -2741,7 +2741,7 @@
         <v>6</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>42</v>
@@ -2774,7 +2774,7 @@
       </c>
       <c r="D51" s="14"/>
       <c r="F51" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>42</v>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="D52" s="14"/>
       <c r="F52" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>42</v>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="F53" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>42</v>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="D54" s="28"/>
       <c r="F54" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>42</v>
@@ -2941,12 +2941,12 @@
       <c r="D59"/>
     </row>
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="87" t="s">
-        <v>184</v>
-      </c>
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
+      <c r="A60" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="95"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="95"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
@@ -3030,7 +3030,7 @@
         <v>32</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D67" s="14"/>
     </row>
@@ -3042,7 +3042,7 @@
         <v>32</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D68" s="2"/>
     </row>
@@ -3057,12 +3057,12 @@
       <c r="D70"/>
     </row>
     <row r="71" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="87" t="s">
+      <c r="A71" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="88"/>
-      <c r="C71" s="88"/>
-      <c r="D71" s="88"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="95"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="23" t="s">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="D73" s="14"/>
       <c r="F73" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G73" s="41" t="s">
         <v>39</v>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="D74" s="14"/>
       <c r="F74" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G74" s="41" t="s">
         <v>39</v>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="D75" s="14"/>
       <c r="F75" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G75" s="41" t="s">
         <v>39</v>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="D76" s="28"/>
       <c r="F76" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G76" s="41" t="s">
         <v>39</v>
@@ -3257,14 +3257,14 @@
         <v>30</v>
       </c>
       <c r="D77" s="28"/>
-      <c r="F77" s="93"/>
-      <c r="G77" s="95"/>
-      <c r="H77" s="95"/>
-      <c r="I77" s="96"/>
-      <c r="J77" s="95"/>
-      <c r="K77" s="95"/>
-      <c r="L77" s="95"/>
-      <c r="M77" s="97"/>
+      <c r="F77" s="88"/>
+      <c r="G77" s="90"/>
+      <c r="H77" s="90"/>
+      <c r="I77" s="91"/>
+      <c r="J77" s="90"/>
+      <c r="K77" s="90"/>
+      <c r="L77" s="90"/>
+      <c r="M77" s="92"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
@@ -3277,14 +3277,14 @@
         <v>95</v>
       </c>
       <c r="D78" s="14"/>
-      <c r="F78" s="93"/>
-      <c r="G78" s="95"/>
-      <c r="H78" s="95"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="95"/>
-      <c r="K78" s="95"/>
-      <c r="L78" s="98"/>
-      <c r="M78" s="97"/>
+      <c r="F78" s="88"/>
+      <c r="G78" s="90"/>
+      <c r="H78" s="90"/>
+      <c r="I78" s="91"/>
+      <c r="J78" s="90"/>
+      <c r="K78" s="90"/>
+      <c r="L78" s="93"/>
+      <c r="M78" s="92"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
@@ -3297,14 +3297,14 @@
         <v>96</v>
       </c>
       <c r="D79" s="14"/>
-      <c r="F79" s="93"/>
-      <c r="G79" s="95"/>
-      <c r="H79" s="95"/>
-      <c r="I79" s="96"/>
-      <c r="J79" s="95"/>
-      <c r="K79" s="95"/>
-      <c r="L79" s="95"/>
-      <c r="M79" s="97"/>
+      <c r="F79" s="88"/>
+      <c r="G79" s="90"/>
+      <c r="H79" s="90"/>
+      <c r="I79" s="91"/>
+      <c r="J79" s="90"/>
+      <c r="K79" s="90"/>
+      <c r="L79" s="90"/>
+      <c r="M79" s="92"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
@@ -3317,105 +3317,105 @@
         <v>97</v>
       </c>
       <c r="D80" s="2"/>
-      <c r="F80" s="93"/>
-      <c r="G80" s="95"/>
-      <c r="H80" s="95"/>
-      <c r="I80" s="96"/>
-      <c r="J80" s="95"/>
-      <c r="K80" s="95"/>
-      <c r="L80" s="95"/>
-      <c r="M80" s="97"/>
+      <c r="F80" s="88"/>
+      <c r="G80" s="90"/>
+      <c r="H80" s="90"/>
+      <c r="I80" s="91"/>
+      <c r="J80" s="90"/>
+      <c r="K80" s="90"/>
+      <c r="L80" s="90"/>
+      <c r="M80" s="92"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81"/>
-      <c r="F81" s="93"/>
-      <c r="G81" s="95"/>
-      <c r="H81" s="95"/>
-      <c r="I81" s="96"/>
-      <c r="J81" s="95"/>
-      <c r="K81" s="95"/>
-      <c r="L81" s="98"/>
-      <c r="M81" s="97"/>
+      <c r="F81" s="88"/>
+      <c r="G81" s="90"/>
+      <c r="H81" s="90"/>
+      <c r="I81" s="91"/>
+      <c r="J81" s="90"/>
+      <c r="K81" s="90"/>
+      <c r="L81" s="93"/>
+      <c r="M81" s="92"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82"/>
-      <c r="F82" s="93"/>
-      <c r="G82" s="95"/>
-      <c r="H82" s="95"/>
-      <c r="I82" s="96"/>
-      <c r="J82" s="95"/>
-      <c r="K82" s="95"/>
-      <c r="L82" s="95"/>
-      <c r="M82" s="97"/>
+      <c r="F82" s="88"/>
+      <c r="G82" s="90"/>
+      <c r="H82" s="90"/>
+      <c r="I82" s="91"/>
+      <c r="J82" s="90"/>
+      <c r="K82" s="90"/>
+      <c r="L82" s="90"/>
+      <c r="M82" s="92"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83"/>
-      <c r="F83" s="93"/>
-      <c r="G83" s="95"/>
-      <c r="H83" s="95"/>
-      <c r="I83" s="96"/>
-      <c r="J83" s="95"/>
-      <c r="K83" s="95"/>
-      <c r="L83" s="95"/>
-      <c r="M83" s="97"/>
+      <c r="F83" s="88"/>
+      <c r="G83" s="90"/>
+      <c r="H83" s="90"/>
+      <c r="I83" s="91"/>
+      <c r="J83" s="90"/>
+      <c r="K83" s="90"/>
+      <c r="L83" s="90"/>
+      <c r="M83" s="92"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84"/>
-      <c r="F84" s="93"/>
+      <c r="F84" s="88"/>
       <c r="G84" s="36"/>
       <c r="H84" s="36"/>
-      <c r="I84" s="93"/>
+      <c r="I84" s="88"/>
       <c r="J84" s="36"/>
       <c r="K84" s="36"/>
       <c r="L84" s="36"/>
-      <c r="M84" s="94"/>
+      <c r="M84" s="89"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85"/>
-      <c r="F85" s="93"/>
+      <c r="F85" s="88"/>
       <c r="G85" s="36"/>
       <c r="H85" s="36"/>
-      <c r="I85" s="93"/>
+      <c r="I85" s="88"/>
       <c r="J85" s="36"/>
       <c r="K85" s="36"/>
       <c r="L85" s="36"/>
-      <c r="M85" s="94"/>
+      <c r="M85" s="89"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86"/>
-      <c r="F86" s="93"/>
+      <c r="F86" s="88"/>
       <c r="G86" s="36"/>
       <c r="H86" s="36"/>
-      <c r="I86" s="93"/>
+      <c r="I86" s="88"/>
       <c r="J86" s="36"/>
       <c r="K86" s="36"/>
       <c r="L86" s="36"/>
-      <c r="M86" s="94"/>
+      <c r="M86" s="89"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87"/>
-      <c r="F87" s="93"/>
-      <c r="G87" s="95"/>
-      <c r="H87" s="95"/>
-      <c r="I87" s="95"/>
-      <c r="J87" s="95"/>
-      <c r="K87" s="95"/>
+      <c r="F87" s="88"/>
+      <c r="G87" s="90"/>
+      <c r="H87" s="90"/>
+      <c r="I87" s="90"/>
+      <c r="J87" s="90"/>
+      <c r="K87" s="90"/>
       <c r="L87" s="36"/>
-      <c r="M87" s="94"/>
+      <c r="M87" s="89"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
@@ -3490,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528A46A0-1E4B-49CC-85D9-668A5231DAB9}">
   <dimension ref="A1:Z94"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3517,15 +3517,15 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F1" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
+      <c r="A2" s="97" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
     </row>
     <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="68" t="s">
@@ -3538,10 +3538,10 @@
         <v>5</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>7</v>
@@ -3559,61 +3559,61 @@
         <v>54</v>
       </c>
       <c r="M3" s="49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N3" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="T3" s="49" t="s">
         <v>102</v>
-      </c>
-      <c r="O3" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q3" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="R3" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="S3" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="T3" s="49" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="59"/>
       <c r="F4" s="53">
         <v>43966</v>
       </c>
       <c r="G4" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I4" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K4" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L4" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M4" s="54">
         <v>2</v>
@@ -3642,35 +3642,35 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" s="59"/>
       <c r="F5" s="53">
         <v>43967</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K5" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M5" s="54">
         <v>2</v>
@@ -3702,7 +3702,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>17</v>
@@ -3712,22 +3712,22 @@
         <v>43968</v>
       </c>
       <c r="G6" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I6" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J6" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K6" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M6" s="54">
         <v>2</v>
@@ -3759,7 +3759,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>23</v>
@@ -3769,22 +3769,22 @@
         <v>43969</v>
       </c>
       <c r="G7" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M7" s="54">
         <v>2</v>
@@ -3816,7 +3816,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>27</v>
@@ -3826,22 +3826,22 @@
         <v>43970</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I8" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J8" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M8" s="54">
         <v>2</v>
@@ -3873,7 +3873,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>29</v>
@@ -3886,7 +3886,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>30</v>
@@ -3896,112 +3896,112 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="59"/>
       <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" s="59"/>
       <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="59"/>
       <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="59"/>
       <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="59"/>
       <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="58" t="s">
-        <v>101</v>
-      </c>
       <c r="C17" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="59"/>
       <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="97" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="68" t="s">
@@ -4014,7 +4014,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G22" s="49" t="s">
         <v>7</v>
@@ -4032,78 +4032,78 @@
         <v>54</v>
       </c>
       <c r="L22" s="49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M22" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="N22" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="P22" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q22" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="R22" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="S22" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="N22" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="O22" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="P22" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q22" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="R22" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="S22" s="49" t="s">
-        <v>103</v>
-      </c>
       <c r="T22" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="U22" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="V22" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="W22" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="U22" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="V22" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="W22" s="49" t="s">
-        <v>123</v>
-      </c>
       <c r="X22" s="49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Y22" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z22" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="Z22" s="49" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F23" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J23" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K23" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L23" s="53">
         <v>43954</v>
@@ -4156,28 +4156,28 @@
         <v>7</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I24" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J24" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K24" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L24" s="53">
         <v>44017</v>
@@ -4230,28 +4230,28 @@
         <v>8</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J25" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L25" s="53">
         <v>43989</v>
@@ -4304,28 +4304,28 @@
         <v>9</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G26" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J26" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K26" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L26" s="53">
         <v>43961</v>
@@ -4378,28 +4378,28 @@
         <v>28</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I27" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J27" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K27" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L27" s="53">
         <v>44024</v>
@@ -4452,28 +4452,28 @@
         <v>54</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I28" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J28" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L28" s="53">
         <v>43996</v>
@@ -4523,31 +4523,31 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F29" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G29" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H29" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I29" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J29" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L29" s="53">
         <v>43968</v>
@@ -4597,31 +4597,31 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G30" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H30" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J30" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K30" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L30" s="53">
         <v>44031</v>
@@ -4671,31 +4671,31 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F31" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G31" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H31" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J31" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K31" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L31" s="53">
         <v>44003</v>
@@ -4745,31 +4745,31 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F32" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H32" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I32" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J32" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K32" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L32" s="53">
         <v>43975</v>
@@ -4819,136 +4819,136 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="58" t="s">
-        <v>101</v>
-      </c>
       <c r="C35" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B41" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="91"/>
+      <c r="A45" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="98"/>
+      <c r="C45" s="98"/>
       <c r="F45" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G45" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H45" s="48" t="s">
         <v>7</v>
@@ -4960,10 +4960,10 @@
         <v>9</v>
       </c>
       <c r="K45" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -4980,16 +4980,16 @@
         <v>43960</v>
       </c>
       <c r="G46" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H46" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I46" s="61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J46" s="61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K46" s="54">
         <v>1</v>
@@ -5000,28 +5000,28 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F47" s="60">
         <v>43960</v>
       </c>
       <c r="G47" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H47" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I47" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="61" t="s">
         <v>149</v>
-      </c>
-      <c r="J47" s="61" t="s">
-        <v>151</v>
       </c>
       <c r="K47" s="54">
         <v>1</v>
@@ -5032,28 +5032,28 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F48" s="60">
         <v>43960</v>
       </c>
       <c r="G48" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H48" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I48" s="61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J48" s="61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K48" s="54">
         <v>1</v>
@@ -5067,7 +5067,7 @@
         <v>7</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>17</v>
@@ -5076,16 +5076,16 @@
         <v>43960</v>
       </c>
       <c r="G49" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H49" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I49" s="61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J49" s="61" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K49" s="54">
         <v>1</v>
@@ -5099,7 +5099,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>23</v>
@@ -5110,7 +5110,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>27</v>
@@ -5118,32 +5118,32 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B52" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B53" s="63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="90" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="91"/>
+      <c r="A56" s="97" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="98"/>
+      <c r="C56" s="98"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="68" t="s">
@@ -5156,10 +5156,10 @@
         <v>5</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G57" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H57" s="48" t="s">
         <v>7</v>
@@ -5174,36 +5174,36 @@
         <v>12</v>
       </c>
       <c r="L57" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M57" s="48" t="s">
         <v>38</v>
       </c>
       <c r="N57" s="48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O57" s="48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F58" s="53">
         <v>44019</v>
       </c>
       <c r="G58" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H58" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I58" s="54" t="s">
         <v>39</v>
@@ -5212,7 +5212,7 @@
         <v>39</v>
       </c>
       <c r="K58" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L58" s="54">
         <v>3</v>
@@ -5229,22 +5229,22 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B59" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F59" s="53">
         <v>44020</v>
       </c>
       <c r="G59" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H59" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I59" s="54" t="s">
         <v>39</v>
@@ -5253,7 +5253,7 @@
         <v>39</v>
       </c>
       <c r="K59" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L59" s="54">
         <v>3</v>
@@ -5273,19 +5273,19 @@
         <v>7</v>
       </c>
       <c r="B60" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F60" s="53">
         <v>44021</v>
       </c>
       <c r="G60" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H60" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I60" s="54" t="s">
         <v>39</v>
@@ -5294,7 +5294,7 @@
         <v>39</v>
       </c>
       <c r="K60" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L60" s="54">
         <v>3</v>
@@ -5314,19 +5314,19 @@
         <v>8</v>
       </c>
       <c r="B61" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F61" s="53">
         <v>44022</v>
       </c>
       <c r="G61" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H61" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I61" s="54" t="s">
         <v>39</v>
@@ -5335,7 +5335,7 @@
         <v>39</v>
       </c>
       <c r="K61" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L61" s="54">
         <v>3</v>
@@ -5355,19 +5355,19 @@
         <v>9</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F62" s="53">
         <v>44023</v>
       </c>
       <c r="G62" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H62" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I62" s="54" t="s">
         <v>39</v>
@@ -5376,7 +5376,7 @@
         <v>39</v>
       </c>
       <c r="K62" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L62" s="54">
         <v>3</v>
@@ -5393,22 +5393,22 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F63" s="53">
         <v>44024</v>
       </c>
       <c r="G63" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H63" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I63" s="54" t="s">
         <v>39</v>
@@ -5417,7 +5417,7 @@
         <v>39</v>
       </c>
       <c r="K63" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L63" s="54">
         <v>3</v>
@@ -5437,7 +5437,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>31</v>
@@ -5446,10 +5446,10 @@
         <v>44025</v>
       </c>
       <c r="G64" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H64" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I64" s="54" t="s">
         <v>39</v>
@@ -5458,7 +5458,7 @@
         <v>39</v>
       </c>
       <c r="K64" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L64" s="54">
         <v>3</v>
@@ -5478,47 +5478,47 @@
         <v>38</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="58" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B67" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B68" s="65"/>
       <c r="C68" s="51"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="90" t="s">
-        <v>148</v>
-      </c>
-      <c r="B70" s="91"/>
-      <c r="C70" s="91"/>
+      <c r="A70" s="97" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="46" t="s">
@@ -5531,10 +5531,10 @@
         <v>5</v>
       </c>
       <c r="F71" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H71" s="48" t="s">
         <v>7</v>
@@ -5549,45 +5549,45 @@
         <v>12</v>
       </c>
       <c r="L71" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M71" s="48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N71" s="48" t="s">
         <v>38</v>
       </c>
       <c r="O71" s="48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B72" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C72" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F72" s="53">
         <v>43948</v>
       </c>
       <c r="G72" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H72" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I72" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J72" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K72" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L72" s="54">
         <v>2</v>
@@ -5604,31 +5604,31 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F73" s="53">
         <v>43949</v>
       </c>
       <c r="G73" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H73" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I73" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J73" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K73" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K73" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L73" s="54">
         <v>2</v>
@@ -5648,28 +5648,28 @@
         <v>7</v>
       </c>
       <c r="B74" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F74" s="53">
         <v>43949</v>
       </c>
       <c r="G74" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H74" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I74" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J74" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K74" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L74" s="54">
         <v>2</v>
@@ -5689,7 +5689,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>23</v>
@@ -5698,19 +5698,19 @@
         <v>43950</v>
       </c>
       <c r="G75" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H75" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I75" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J75" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K75" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K75" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L75" s="54">
         <v>2</v>
@@ -5730,7 +5730,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>52</v>
@@ -5739,19 +5739,19 @@
         <v>43950</v>
       </c>
       <c r="G76" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H76" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I76" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J76" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K76" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L76" s="54">
         <v>2</v>
@@ -5768,31 +5768,31 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B77" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F77" s="53">
         <v>43951</v>
       </c>
       <c r="G77" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H77" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I77" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J77" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K77" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K77" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L77" s="54">
         <v>2</v>
@@ -5812,7 +5812,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>31</v>
@@ -5821,13 +5821,13 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="B79" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="F79" s="55"/>
     </row>
@@ -5836,37 +5836,37 @@
         <v>38</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F80" s="55"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B81" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F81" s="55"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F82" s="55"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="90" t="s">
-        <v>238</v>
-      </c>
-      <c r="B85" s="91"/>
-      <c r="C85" s="91"/>
+      <c r="A85" s="97" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="68" t="s">
@@ -5880,36 +5880,36 @@
       </c>
       <c r="D86" s="51"/>
       <c r="F86" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G86" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H86" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I86" s="48" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J86" s="48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L86" s="48" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B87" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D87" s="67"/>
       <c r="E87" s="59"/>
@@ -5917,7 +5917,7 @@
         <v>43948</v>
       </c>
       <c r="G87" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H87" s="54">
         <v>1</v>
@@ -5937,20 +5937,20 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B88" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D88" s="51"/>
       <c r="F88" s="53">
         <v>43949</v>
       </c>
       <c r="G88" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H88" s="54">
         <v>1</v>
@@ -5970,13 +5970,13 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B89" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D89" s="67"/>
       <c r="E89" s="59"/>
@@ -5984,7 +5984,7 @@
         <v>43950</v>
       </c>
       <c r="G89" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H89" s="54">
         <v>1</v>
@@ -6004,13 +6004,13 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="58" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B90" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D90" s="67"/>
       <c r="E90" s="59"/>
@@ -6018,7 +6018,7 @@
         <v>43951</v>
       </c>
       <c r="G90" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H90" s="54">
         <v>1</v>
@@ -6038,13 +6038,13 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B91" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D91" s="67"/>
       <c r="E91" s="59"/>
@@ -6052,7 +6052,7 @@
         <v>43952</v>
       </c>
       <c r="G91" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H91" s="54">
         <v>1</v>
@@ -6072,13 +6072,13 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B92" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D92" s="67"/>
       <c r="E92" s="59"/>
@@ -6086,7 +6086,7 @@
         <v>43953</v>
       </c>
       <c r="G92" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H92" s="54">
         <v>1</v>
@@ -6106,13 +6106,13 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B93" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D93" s="67"/>
       <c r="E93" s="59"/>
@@ -6159,11 +6159,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
+      <c r="A2" s="97" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
       <c r="F2" s="79" t="s">
         <v>7</v>
       </c>
@@ -6180,10 +6180,10 @@
         <v>28</v>
       </c>
       <c r="K2" s="79" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L2" s="79" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -6197,16 +6197,16 @@
         <v>5</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>55</v>
@@ -6223,22 +6223,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>55</v>
@@ -6255,22 +6255,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>55</v>
@@ -6287,22 +6287,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>55</v>
@@ -6319,22 +6319,22 @@
         <v>28</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>55</v>
@@ -6351,22 +6351,22 @@
         <v>54</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>55</v>
@@ -6380,25 +6380,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="63" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>191</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>55</v>
@@ -6412,25 +6412,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>55</v>
@@ -6444,16 +6444,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F11" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>55</v>
@@ -6467,12 +6467,12 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -6507,11 +6507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="A1" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="68" t="s">
@@ -6524,7 +6524,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G2" s="79" t="s">
         <v>7</v>
@@ -6545,36 +6545,36 @@
         <v>12</v>
       </c>
       <c r="M2" s="79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -6584,7 +6584,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
@@ -6593,19 +6593,19 @@
         <v>58</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>199</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -6615,7 +6615,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>23</v>
@@ -6624,19 +6624,19 @@
         <v>58</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -6646,7 +6646,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>27</v>
@@ -6655,19 +6655,19 @@
         <v>58</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -6677,7 +6677,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>29</v>
@@ -6686,19 +6686,19 @@
         <v>58</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>204</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -6708,7 +6708,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
@@ -6717,19 +6717,19 @@
         <v>58</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -6748,19 +6748,19 @@
         <v>58</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -6779,19 +6779,19 @@
         <v>58</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -6801,29 +6801,29 @@
         <v>58</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="90" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="97" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
       <c r="F13" s="48" t="s">
         <v>7</v>
       </c>
@@ -6840,16 +6840,16 @@
         <v>54</v>
       </c>
       <c r="K13" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="M13" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="L13" s="48" t="s">
+      <c r="N13" s="48" t="s">
         <v>209</v>
-      </c>
-      <c r="M13" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="N13" s="48" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -6863,7 +6863,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>18</v>
@@ -6875,7 +6875,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K14" s="32">
         <v>0</v>
@@ -6895,13 +6895,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="76" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>18</v>
@@ -6913,7 +6913,7 @@
         <v>55</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K15" s="32">
         <v>0</v>
@@ -6933,25 +6933,25 @@
         <v>8</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="71" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K16" s="32">
         <v>0</v>
@@ -6971,25 +6971,25 @@
         <v>9</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="71" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I17" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K17" s="32">
         <v>0</v>
@@ -7009,25 +7009,25 @@
         <v>28</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="71" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I18" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K18" s="32">
         <v>0</v>
@@ -7047,25 +7047,25 @@
         <v>54</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="71" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I19" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K19" s="32">
         <v>0</v>
@@ -7082,28 +7082,28 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="70" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I20" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K20" s="32">
         <v>0</v>
@@ -7120,28 +7120,28 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="70" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B21" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I21" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K21" s="32">
         <v>0</v>
@@ -7158,28 +7158,28 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I22" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K22" s="32">
         <v>0</v>
@@ -7196,28 +7196,28 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I23" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K23" s="32">
         <v>0</v>
@@ -7234,15 +7234,15 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F24" s="80" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="90" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
+      <c r="A27" s="97" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
       <c r="F27" s="79" t="s">
         <v>7</v>
       </c>
@@ -7256,10 +7256,10 @@
         <v>12</v>
       </c>
       <c r="J27" s="79" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K27" s="79" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -7273,7 +7273,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>39</v>
@@ -7282,7 +7282,7 @@
         <v>39</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J28" s="8">
         <v>0</v>
@@ -7296,13 +7296,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>18</v>
@@ -7311,7 +7311,7 @@
         <v>24</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J29" s="8">
         <v>1</v>
@@ -7325,22 +7325,22 @@
         <v>8</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="83" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J30" s="8">
         <v>1</v>
@@ -7354,22 +7354,22 @@
         <v>9</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="83" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J31" s="8">
         <v>1</v>
@@ -7383,22 +7383,22 @@
         <v>12</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="83" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J32" s="8">
         <v>1</v>
@@ -7409,25 +7409,25 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="84" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B33" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J33" s="8">
         <v>1</v>
@@ -7438,21 +7438,21 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="84" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B34" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F34" s="74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F35" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -7469,6 +7469,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F33A6DB98216B5448738561EEB5E52F3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b9409f311f3f1f262294d1b1bffdd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cc8eddb-c4fa-487b-b5b5-3b55fe26257b" xmlns:ns3="d3a4b13c-8f4e-44e8-9732-bc540be98408" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bff76ea5e37bf585a119dc8c50450aee" ns2:_="" ns3:_="">
     <xsd:import namespace="2cc8eddb-c4fa-487b-b5b5-3b55fe26257b"/>
@@ -7679,22 +7694,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CC594F-C037-4148-B9F5-575D82E062CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE803B83-899C-4D1E-8DBC-13369AC549E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6DE800C-9F6D-468E-B968-BE9FB6D7D6B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7711,21 +7728,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE803B83-899C-4D1E-8DBC-13369AC549E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CC594F-C037-4148-B9F5-575D82E062CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pulling latest updates from public GitHub.
</commit_message>
<xml_diff>
--- a/mro_documentation/mro_or_data_model.xlsx
+++ b/mro_documentation/mro_or_data_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\casuser\Cleveland_Clinic\gitbackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\casuser\Cleveland_Clinic\gitrepo\mro_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AB8CC6-D584-420E-B7E4-4F127A7473DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C35148-3EF2-43B1-A2E7-FAC55ACD2533}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS FOR OPTIMIZATION" sheetId="1" r:id="rId1"/>
@@ -333,9 +333,6 @@
     <t>Vascular Services</t>
   </si>
   <si>
-    <t>OUTPUT_OPT_DETAIL</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
   </si>
   <si>
     <t xml:space="preserve">Number of new patients admitted without the COVID-19 testing requirements </t>
-  </si>
-  <si>
-    <t>OUTPUT_OPT_DETAIL_AGG</t>
   </si>
   <si>
     <t>DailyDemand</t>
@@ -770,6 +764,12 @@
   </si>
   <si>
     <t>Facilty2</t>
+  </si>
+  <si>
+    <t>OUTPUT_OPT_DETAIL_DAILY</t>
+  </si>
+  <si>
+    <t>OUTPUT_OPT_DETAIL_WEEKLY</t>
   </si>
 </sst>
 </file>
@@ -1305,6 +1305,21 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1318,21 +1333,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1652,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1675,29 +1675,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="F2" s="89" t="s">
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="F2" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="D6" s="8"/>
       <c r="F6" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>18</v>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="F7" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>18</v>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="F8" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>18</v>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="D9" s="8"/>
       <c r="F9" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>18</v>
@@ -1967,12 +1967,12 @@
       <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="88"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
       <c r="M16" s="21"/>
       <c r="N16" s="27"/>
     </row>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="D18" s="8"/>
       <c r="F18" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>39</v>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="D19" s="8"/>
       <c r="F19" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>39</v>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="F20" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>42</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="F21" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>42</v>
@@ -2145,12 +2145,12 @@
       <c r="N23" s="27"/>
     </row>
     <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="87" t="s">
+      <c r="A24" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="88"/>
-      <c r="C24" s="88"/>
-      <c r="D24" s="88"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
       <c r="M24" s="21"/>
       <c r="N24" s="27"/>
     </row>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="D26" s="9"/>
       <c r="F26" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>18</v>
@@ -2215,10 +2215,10 @@
       <c r="J26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="92">
+      <c r="K26" s="87">
         <v>10000</v>
       </c>
-      <c r="L26" s="92">
+      <c r="L26" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D27" s="7"/>
       <c r="F27" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>18</v>
@@ -2248,10 +2248,10 @@
       <c r="J27" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K27" s="92">
+      <c r="K27" s="87">
         <v>10000</v>
       </c>
-      <c r="L27" s="92">
+      <c r="L27" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="F28" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>18</v>
@@ -2281,10 +2281,10 @@
       <c r="J28" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="92">
+      <c r="K28" s="87">
         <v>10000</v>
       </c>
-      <c r="L28" s="92">
+      <c r="L28" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="D29" s="7"/>
       <c r="F29" s="32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>18</v>
@@ -2314,10 +2314,10 @@
       <c r="J29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K29" s="92">
+      <c r="K29" s="87">
         <v>10000</v>
       </c>
-      <c r="L29" s="92">
+      <c r="L29" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="D30" s="7"/>
       <c r="F30" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>18</v>
@@ -2347,10 +2347,10 @@
       <c r="J30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K30" s="92">
+      <c r="K30" s="87">
         <v>10000</v>
       </c>
-      <c r="L30" s="92">
+      <c r="L30" s="87">
         <v>1000</v>
       </c>
     </row>
@@ -2383,12 +2383,12 @@
       <c r="F33"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="87" t="s">
+      <c r="A34" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="88"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
+      <c r="B34" s="95"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="95"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="D36" s="9"/>
       <c r="F36" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>42</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="F37" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>42</v>
@@ -2699,14 +2699,14 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="87" t="s">
+      <c r="A49" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="88"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="88"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
       <c r="F49" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>42</v>
@@ -2741,7 +2741,7 @@
         <v>6</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>42</v>
@@ -2774,7 +2774,7 @@
       </c>
       <c r="D51" s="14"/>
       <c r="F51" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>42</v>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="D52" s="14"/>
       <c r="F52" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>42</v>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="F53" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>42</v>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="D54" s="28"/>
       <c r="F54" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>42</v>
@@ -2941,12 +2941,12 @@
       <c r="D59"/>
     </row>
     <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="87" t="s">
-        <v>184</v>
-      </c>
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
+      <c r="A60" s="94" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="95"/>
+      <c r="C60" s="95"/>
+      <c r="D60" s="95"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
@@ -3030,7 +3030,7 @@
         <v>32</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D67" s="14"/>
     </row>
@@ -3042,7 +3042,7 @@
         <v>32</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D68" s="2"/>
     </row>
@@ -3057,12 +3057,12 @@
       <c r="D70"/>
     </row>
     <row r="71" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="87" t="s">
+      <c r="A71" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="88"/>
-      <c r="C71" s="88"/>
-      <c r="D71" s="88"/>
+      <c r="B71" s="95"/>
+      <c r="C71" s="95"/>
+      <c r="D71" s="95"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="23" t="s">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="D73" s="14"/>
       <c r="F73" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G73" s="41" t="s">
         <v>39</v>
@@ -3150,7 +3150,7 @@
       </c>
       <c r="D74" s="14"/>
       <c r="F74" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G74" s="41" t="s">
         <v>39</v>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="D75" s="14"/>
       <c r="F75" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G75" s="41" t="s">
         <v>39</v>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="D76" s="28"/>
       <c r="F76" s="32" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G76" s="41" t="s">
         <v>39</v>
@@ -3257,14 +3257,14 @@
         <v>30</v>
       </c>
       <c r="D77" s="28"/>
-      <c r="F77" s="93"/>
-      <c r="G77" s="95"/>
-      <c r="H77" s="95"/>
-      <c r="I77" s="96"/>
-      <c r="J77" s="95"/>
-      <c r="K77" s="95"/>
-      <c r="L77" s="95"/>
-      <c r="M77" s="97"/>
+      <c r="F77" s="88"/>
+      <c r="G77" s="90"/>
+      <c r="H77" s="90"/>
+      <c r="I77" s="91"/>
+      <c r="J77" s="90"/>
+      <c r="K77" s="90"/>
+      <c r="L77" s="90"/>
+      <c r="M77" s="92"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
@@ -3277,14 +3277,14 @@
         <v>95</v>
       </c>
       <c r="D78" s="14"/>
-      <c r="F78" s="93"/>
-      <c r="G78" s="95"/>
-      <c r="H78" s="95"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="95"/>
-      <c r="K78" s="95"/>
-      <c r="L78" s="98"/>
-      <c r="M78" s="97"/>
+      <c r="F78" s="88"/>
+      <c r="G78" s="90"/>
+      <c r="H78" s="90"/>
+      <c r="I78" s="91"/>
+      <c r="J78" s="90"/>
+      <c r="K78" s="90"/>
+      <c r="L78" s="93"/>
+      <c r="M78" s="92"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
@@ -3297,14 +3297,14 @@
         <v>96</v>
       </c>
       <c r="D79" s="14"/>
-      <c r="F79" s="93"/>
-      <c r="G79" s="95"/>
-      <c r="H79" s="95"/>
-      <c r="I79" s="96"/>
-      <c r="J79" s="95"/>
-      <c r="K79" s="95"/>
-      <c r="L79" s="95"/>
-      <c r="M79" s="97"/>
+      <c r="F79" s="88"/>
+      <c r="G79" s="90"/>
+      <c r="H79" s="90"/>
+      <c r="I79" s="91"/>
+      <c r="J79" s="90"/>
+      <c r="K79" s="90"/>
+      <c r="L79" s="90"/>
+      <c r="M79" s="92"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
@@ -3317,105 +3317,105 @@
         <v>97</v>
       </c>
       <c r="D80" s="2"/>
-      <c r="F80" s="93"/>
-      <c r="G80" s="95"/>
-      <c r="H80" s="95"/>
-      <c r="I80" s="96"/>
-      <c r="J80" s="95"/>
-      <c r="K80" s="95"/>
-      <c r="L80" s="95"/>
-      <c r="M80" s="97"/>
+      <c r="F80" s="88"/>
+      <c r="G80" s="90"/>
+      <c r="H80" s="90"/>
+      <c r="I80" s="91"/>
+      <c r="J80" s="90"/>
+      <c r="K80" s="90"/>
+      <c r="L80" s="90"/>
+      <c r="M80" s="92"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81"/>
-      <c r="F81" s="93"/>
-      <c r="G81" s="95"/>
-      <c r="H81" s="95"/>
-      <c r="I81" s="96"/>
-      <c r="J81" s="95"/>
-      <c r="K81" s="95"/>
-      <c r="L81" s="98"/>
-      <c r="M81" s="97"/>
+      <c r="F81" s="88"/>
+      <c r="G81" s="90"/>
+      <c r="H81" s="90"/>
+      <c r="I81" s="91"/>
+      <c r="J81" s="90"/>
+      <c r="K81" s="90"/>
+      <c r="L81" s="93"/>
+      <c r="M81" s="92"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82"/>
-      <c r="F82" s="93"/>
-      <c r="G82" s="95"/>
-      <c r="H82" s="95"/>
-      <c r="I82" s="96"/>
-      <c r="J82" s="95"/>
-      <c r="K82" s="95"/>
-      <c r="L82" s="95"/>
-      <c r="M82" s="97"/>
+      <c r="F82" s="88"/>
+      <c r="G82" s="90"/>
+      <c r="H82" s="90"/>
+      <c r="I82" s="91"/>
+      <c r="J82" s="90"/>
+      <c r="K82" s="90"/>
+      <c r="L82" s="90"/>
+      <c r="M82" s="92"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83"/>
-      <c r="F83" s="93"/>
-      <c r="G83" s="95"/>
-      <c r="H83" s="95"/>
-      <c r="I83" s="96"/>
-      <c r="J83" s="95"/>
-      <c r="K83" s="95"/>
-      <c r="L83" s="95"/>
-      <c r="M83" s="97"/>
+      <c r="F83" s="88"/>
+      <c r="G83" s="90"/>
+      <c r="H83" s="90"/>
+      <c r="I83" s="91"/>
+      <c r="J83" s="90"/>
+      <c r="K83" s="90"/>
+      <c r="L83" s="90"/>
+      <c r="M83" s="92"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84"/>
-      <c r="F84" s="93"/>
+      <c r="F84" s="88"/>
       <c r="G84" s="36"/>
       <c r="H84" s="36"/>
-      <c r="I84" s="93"/>
+      <c r="I84" s="88"/>
       <c r="J84" s="36"/>
       <c r="K84" s="36"/>
       <c r="L84" s="36"/>
-      <c r="M84" s="94"/>
+      <c r="M84" s="89"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85"/>
-      <c r="F85" s="93"/>
+      <c r="F85" s="88"/>
       <c r="G85" s="36"/>
       <c r="H85" s="36"/>
-      <c r="I85" s="93"/>
+      <c r="I85" s="88"/>
       <c r="J85" s="36"/>
       <c r="K85" s="36"/>
       <c r="L85" s="36"/>
-      <c r="M85" s="94"/>
+      <c r="M85" s="89"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86"/>
-      <c r="F86" s="93"/>
+      <c r="F86" s="88"/>
       <c r="G86" s="36"/>
       <c r="H86" s="36"/>
-      <c r="I86" s="93"/>
+      <c r="I86" s="88"/>
       <c r="J86" s="36"/>
       <c r="K86" s="36"/>
       <c r="L86" s="36"/>
-      <c r="M86" s="94"/>
+      <c r="M86" s="89"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87"/>
-      <c r="F87" s="93"/>
-      <c r="G87" s="95"/>
-      <c r="H87" s="95"/>
-      <c r="I87" s="95"/>
-      <c r="J87" s="95"/>
-      <c r="K87" s="95"/>
+      <c r="F87" s="88"/>
+      <c r="G87" s="90"/>
+      <c r="H87" s="90"/>
+      <c r="I87" s="90"/>
+      <c r="J87" s="90"/>
+      <c r="K87" s="90"/>
       <c r="L87" s="36"/>
-      <c r="M87" s="94"/>
+      <c r="M87" s="89"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
@@ -3490,8 +3490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528A46A0-1E4B-49CC-85D9-668A5231DAB9}">
   <dimension ref="A1:Z94"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3517,15 +3517,15 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F1" s="45" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
+      <c r="A2" s="97" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
     </row>
     <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="68" t="s">
@@ -3538,10 +3538,10 @@
         <v>5</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>7</v>
@@ -3559,61 +3559,61 @@
         <v>54</v>
       </c>
       <c r="M3" s="49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N3" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="T3" s="49" t="s">
         <v>102</v>
-      </c>
-      <c r="O3" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q3" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="R3" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="S3" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="T3" s="49" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="59"/>
       <c r="F4" s="53">
         <v>43966</v>
       </c>
       <c r="G4" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I4" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K4" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L4" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M4" s="54">
         <v>2</v>
@@ -3642,35 +3642,35 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" s="59"/>
       <c r="F5" s="53">
         <v>43967</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K5" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M5" s="54">
         <v>2</v>
@@ -3702,7 +3702,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>17</v>
@@ -3712,22 +3712,22 @@
         <v>43968</v>
       </c>
       <c r="G6" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I6" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J6" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K6" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M6" s="54">
         <v>2</v>
@@ -3759,7 +3759,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>23</v>
@@ -3769,22 +3769,22 @@
         <v>43969</v>
       </c>
       <c r="G7" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J7" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K7" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M7" s="54">
         <v>2</v>
@@ -3816,7 +3816,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>27</v>
@@ -3826,22 +3826,22 @@
         <v>43970</v>
       </c>
       <c r="G8" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I8" s="54" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J8" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K8" s="54" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M8" s="54">
         <v>2</v>
@@ -3873,7 +3873,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>29</v>
@@ -3886,7 +3886,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>30</v>
@@ -3896,112 +3896,112 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" s="59"/>
       <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" s="59"/>
       <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="59"/>
       <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="59"/>
       <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E16" s="59"/>
       <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="58" t="s">
-        <v>101</v>
-      </c>
       <c r="C17" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="59"/>
       <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="97" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="98"/>
+      <c r="C21" s="98"/>
     </row>
     <row r="22" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="68" t="s">
@@ -4014,7 +4014,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G22" s="49" t="s">
         <v>7</v>
@@ -4032,78 +4032,78 @@
         <v>54</v>
       </c>
       <c r="L22" s="49" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M22" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="N22" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="P22" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q22" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="R22" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="S22" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="N22" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="O22" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="P22" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q22" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="R22" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="S22" s="49" t="s">
-        <v>103</v>
-      </c>
       <c r="T22" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="U22" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="V22" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="W22" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="U22" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="V22" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="W22" s="49" t="s">
-        <v>123</v>
-      </c>
       <c r="X22" s="49" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Y22" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z22" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="Z22" s="49" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F23" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H23" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J23" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K23" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L23" s="53">
         <v>43954</v>
@@ -4156,28 +4156,28 @@
         <v>7</v>
       </c>
       <c r="B24" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I24" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J24" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K24" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L24" s="53">
         <v>44017</v>
@@ -4230,28 +4230,28 @@
         <v>8</v>
       </c>
       <c r="B25" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F25" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J25" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K25" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L25" s="53">
         <v>43989</v>
@@ -4304,28 +4304,28 @@
         <v>9</v>
       </c>
       <c r="B26" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G26" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H26" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J26" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K26" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L26" s="53">
         <v>43961</v>
@@ -4378,28 +4378,28 @@
         <v>28</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H27" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I27" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J27" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K27" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L27" s="53">
         <v>44024</v>
@@ -4452,28 +4452,28 @@
         <v>54</v>
       </c>
       <c r="B28" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H28" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I28" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J28" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K28" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L28" s="53">
         <v>43996</v>
@@ -4523,31 +4523,31 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F29" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G29" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H29" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I29" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J29" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K29" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L29" s="53">
         <v>43968</v>
@@ -4597,31 +4597,31 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F30" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G30" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H30" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J30" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K30" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L30" s="53">
         <v>44031</v>
@@ -4671,31 +4671,31 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F31" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G31" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H31" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J31" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K31" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L31" s="53">
         <v>44003</v>
@@ -4745,31 +4745,31 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F32" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H32" s="54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I32" s="54" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J32" s="54" t="s">
         <v>55</v>
       </c>
       <c r="K32" s="54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L32" s="53">
         <v>43975</v>
@@ -4819,136 +4819,136 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B35" s="58" t="s">
-        <v>101</v>
-      </c>
       <c r="C35" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B38" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" s="58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="58" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B40" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B41" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="58" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="91"/>
+      <c r="A45" s="97" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="98"/>
+      <c r="C45" s="98"/>
       <c r="F45" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G45" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H45" s="48" t="s">
         <v>7</v>
@@ -4960,10 +4960,10 @@
         <v>9</v>
       </c>
       <c r="K45" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -4980,16 +4980,16 @@
         <v>43960</v>
       </c>
       <c r="G46" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H46" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I46" s="61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J46" s="61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K46" s="54">
         <v>1</v>
@@ -5000,28 +5000,28 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" s="58" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F47" s="60">
         <v>43960</v>
       </c>
       <c r="G47" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H47" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I47" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="61" t="s">
         <v>149</v>
-      </c>
-      <c r="J47" s="61" t="s">
-        <v>151</v>
       </c>
       <c r="K47" s="54">
         <v>1</v>
@@ -5032,28 +5032,28 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F48" s="60">
         <v>43960</v>
       </c>
       <c r="G48" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H48" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I48" s="61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J48" s="61" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K48" s="54">
         <v>1</v>
@@ -5067,7 +5067,7 @@
         <v>7</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>17</v>
@@ -5076,16 +5076,16 @@
         <v>43960</v>
       </c>
       <c r="G49" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H49" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I49" s="61" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J49" s="61" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K49" s="54">
         <v>1</v>
@@ -5099,7 +5099,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>23</v>
@@ -5110,7 +5110,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>27</v>
@@ -5118,32 +5118,32 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B52" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B53" s="63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" s="57" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A56" s="90" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" s="91"/>
-      <c r="C56" s="91"/>
+      <c r="A56" s="97" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="98"/>
+      <c r="C56" s="98"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="68" t="s">
@@ -5156,10 +5156,10 @@
         <v>5</v>
       </c>
       <c r="F57" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G57" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H57" s="48" t="s">
         <v>7</v>
@@ -5174,36 +5174,36 @@
         <v>12</v>
       </c>
       <c r="L57" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M57" s="48" t="s">
         <v>38</v>
       </c>
       <c r="N57" s="48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="O57" s="48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F58" s="53">
         <v>44019</v>
       </c>
       <c r="G58" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H58" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I58" s="54" t="s">
         <v>39</v>
@@ -5212,7 +5212,7 @@
         <v>39</v>
       </c>
       <c r="K58" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L58" s="54">
         <v>3</v>
@@ -5229,22 +5229,22 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B59" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F59" s="53">
         <v>44020</v>
       </c>
       <c r="G59" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H59" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I59" s="54" t="s">
         <v>39</v>
@@ -5253,7 +5253,7 @@
         <v>39</v>
       </c>
       <c r="K59" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L59" s="54">
         <v>3</v>
@@ -5273,19 +5273,19 @@
         <v>7</v>
       </c>
       <c r="B60" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F60" s="53">
         <v>44021</v>
       </c>
       <c r="G60" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H60" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I60" s="54" t="s">
         <v>39</v>
@@ -5294,7 +5294,7 @@
         <v>39</v>
       </c>
       <c r="K60" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L60" s="54">
         <v>3</v>
@@ -5314,19 +5314,19 @@
         <v>8</v>
       </c>
       <c r="B61" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F61" s="53">
         <v>44022</v>
       </c>
       <c r="G61" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H61" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I61" s="54" t="s">
         <v>39</v>
@@ -5335,7 +5335,7 @@
         <v>39</v>
       </c>
       <c r="K61" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L61" s="54">
         <v>3</v>
@@ -5355,19 +5355,19 @@
         <v>9</v>
       </c>
       <c r="B62" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F62" s="53">
         <v>44023</v>
       </c>
       <c r="G62" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H62" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I62" s="54" t="s">
         <v>39</v>
@@ -5376,7 +5376,7 @@
         <v>39</v>
       </c>
       <c r="K62" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L62" s="54">
         <v>3</v>
@@ -5393,22 +5393,22 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B63" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F63" s="53">
         <v>44024</v>
       </c>
       <c r="G63" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H63" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I63" s="54" t="s">
         <v>39</v>
@@ -5417,7 +5417,7 @@
         <v>39</v>
       </c>
       <c r="K63" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L63" s="54">
         <v>3</v>
@@ -5437,7 +5437,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>31</v>
@@ -5446,10 +5446,10 @@
         <v>44025</v>
       </c>
       <c r="G64" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H64" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I64" s="54" t="s">
         <v>39</v>
@@ -5458,7 +5458,7 @@
         <v>39</v>
       </c>
       <c r="K64" s="54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L64" s="54">
         <v>3</v>
@@ -5478,47 +5478,47 @@
         <v>38</v>
       </c>
       <c r="B65" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="58" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B66" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B67" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B68" s="65"/>
       <c r="C68" s="51"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="90" t="s">
-        <v>148</v>
-      </c>
-      <c r="B70" s="91"/>
-      <c r="C70" s="91"/>
+      <c r="A70" s="97" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="98"/>
+      <c r="C70" s="98"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="46" t="s">
@@ -5531,10 +5531,10 @@
         <v>5</v>
       </c>
       <c r="F71" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H71" s="48" t="s">
         <v>7</v>
@@ -5549,45 +5549,45 @@
         <v>12</v>
       </c>
       <c r="L71" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M71" s="48" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="N71" s="48" t="s">
         <v>38</v>
       </c>
       <c r="O71" s="48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B72" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C72" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F72" s="53">
         <v>43948</v>
       </c>
       <c r="G72" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H72" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I72" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J72" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K72" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L72" s="54">
         <v>2</v>
@@ -5604,31 +5604,31 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B73" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F73" s="53">
         <v>43949</v>
       </c>
       <c r="G73" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H73" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I73" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J73" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K73" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K73" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L73" s="54">
         <v>2</v>
@@ -5648,28 +5648,28 @@
         <v>7</v>
       </c>
       <c r="B74" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F74" s="53">
         <v>43949</v>
       </c>
       <c r="G74" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H74" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I74" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J74" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K74" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L74" s="54">
         <v>2</v>
@@ -5689,7 +5689,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C75" s="11" t="s">
         <v>23</v>
@@ -5698,19 +5698,19 @@
         <v>43950</v>
       </c>
       <c r="G75" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H75" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I75" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J75" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K75" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K75" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L75" s="54">
         <v>2</v>
@@ -5730,7 +5730,7 @@
         <v>9</v>
       </c>
       <c r="B76" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C76" s="11" t="s">
         <v>52</v>
@@ -5739,19 +5739,19 @@
         <v>43950</v>
       </c>
       <c r="G76" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H76" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I76" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J76" s="54" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K76" s="54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L76" s="54">
         <v>2</v>
@@ -5768,31 +5768,31 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="64" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B77" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F77" s="53">
         <v>43951</v>
       </c>
       <c r="G77" s="54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H77" s="54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I77" s="54" t="s">
         <v>98</v>
       </c>
       <c r="J77" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="K77" s="54" t="s">
         <v>172</v>
-      </c>
-      <c r="K77" s="54" t="s">
-        <v>174</v>
       </c>
       <c r="L77" s="54">
         <v>2</v>
@@ -5812,7 +5812,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>31</v>
@@ -5821,13 +5821,13 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="B79" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>139</v>
-      </c>
-      <c r="B79" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="F79" s="55"/>
     </row>
@@ -5836,37 +5836,37 @@
         <v>38</v>
       </c>
       <c r="B80" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F80" s="55"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B81" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F81" s="55"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F82" s="55"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="90" t="s">
-        <v>238</v>
-      </c>
-      <c r="B85" s="91"/>
-      <c r="C85" s="91"/>
+      <c r="A85" s="97" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" s="98"/>
+      <c r="C85" s="98"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="68" t="s">
@@ -5880,36 +5880,36 @@
       </c>
       <c r="D86" s="51"/>
       <c r="F86" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G86" s="48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H86" s="48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I86" s="48" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J86" s="48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K86" s="48" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L86" s="48" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B87" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D87" s="67"/>
       <c r="E87" s="59"/>
@@ -5917,7 +5917,7 @@
         <v>43948</v>
       </c>
       <c r="G87" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H87" s="54">
         <v>1</v>
@@ -5937,20 +5937,20 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B88" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D88" s="51"/>
       <c r="F88" s="53">
         <v>43949</v>
       </c>
       <c r="G88" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H88" s="54">
         <v>1</v>
@@ -5970,13 +5970,13 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B89" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D89" s="67"/>
       <c r="E89" s="59"/>
@@ -5984,7 +5984,7 @@
         <v>43950</v>
       </c>
       <c r="G89" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H89" s="54">
         <v>1</v>
@@ -6004,13 +6004,13 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="58" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B90" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D90" s="67"/>
       <c r="E90" s="59"/>
@@ -6018,7 +6018,7 @@
         <v>43951</v>
       </c>
       <c r="G90" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H90" s="54">
         <v>1</v>
@@ -6038,13 +6038,13 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B91" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D91" s="67"/>
       <c r="E91" s="59"/>
@@ -6052,7 +6052,7 @@
         <v>43952</v>
       </c>
       <c r="G91" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H91" s="54">
         <v>1</v>
@@ -6072,13 +6072,13 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B92" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D92" s="67"/>
       <c r="E92" s="59"/>
@@ -6086,7 +6086,7 @@
         <v>43953</v>
       </c>
       <c r="G92" s="54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H92" s="54">
         <v>1</v>
@@ -6106,13 +6106,13 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B93" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D93" s="67"/>
       <c r="E93" s="59"/>
@@ -6159,11 +6159,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
+      <c r="A2" s="97" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
       <c r="F2" s="79" t="s">
         <v>7</v>
       </c>
@@ -6180,10 +6180,10 @@
         <v>28</v>
       </c>
       <c r="K2" s="79" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L2" s="79" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -6197,16 +6197,16 @@
         <v>5</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>55</v>
@@ -6223,22 +6223,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>55</v>
@@ -6255,22 +6255,22 @@
         <v>8</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>55</v>
@@ -6287,22 +6287,22 @@
         <v>9</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>55</v>
@@ -6319,22 +6319,22 @@
         <v>28</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>55</v>
@@ -6351,22 +6351,22 @@
         <v>54</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>55</v>
@@ -6380,25 +6380,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="71" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="63" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>191</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>55</v>
@@ -6412,25 +6412,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="70" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>55</v>
@@ -6444,16 +6444,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F11" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>55</v>
@@ -6467,12 +6467,12 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -6507,11 +6507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="A1" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="68" t="s">
@@ -6524,7 +6524,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G2" s="79" t="s">
         <v>7</v>
@@ -6545,36 +6545,36 @@
         <v>12</v>
       </c>
       <c r="M2" s="79" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -6584,7 +6584,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>17</v>
@@ -6593,19 +6593,19 @@
         <v>58</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>199</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
@@ -6615,7 +6615,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>23</v>
@@ -6624,19 +6624,19 @@
         <v>58</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -6646,7 +6646,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>27</v>
@@ -6655,19 +6655,19 @@
         <v>58</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -6677,7 +6677,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>29</v>
@@ -6686,19 +6686,19 @@
         <v>58</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>202</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>204</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -6708,7 +6708,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
@@ -6717,19 +6717,19 @@
         <v>58</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
@@ -6748,19 +6748,19 @@
         <v>58</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -6779,19 +6779,19 @@
         <v>58</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -6801,29 +6801,29 @@
         <v>58</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>55</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="90" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="97" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
       <c r="F13" s="48" t="s">
         <v>7</v>
       </c>
@@ -6840,16 +6840,16 @@
         <v>54</v>
       </c>
       <c r="K13" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="M13" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="L13" s="48" t="s">
+      <c r="N13" s="48" t="s">
         <v>209</v>
-      </c>
-      <c r="M13" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="N13" s="48" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -6863,7 +6863,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G14" s="32" t="s">
         <v>18</v>
@@ -6875,7 +6875,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K14" s="32">
         <v>0</v>
@@ -6895,13 +6895,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="76" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G15" s="32" t="s">
         <v>18</v>
@@ -6913,7 +6913,7 @@
         <v>55</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K15" s="32">
         <v>0</v>
@@ -6933,25 +6933,25 @@
         <v>8</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="71" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H16" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K16" s="32">
         <v>0</v>
@@ -6971,25 +6971,25 @@
         <v>9</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="71" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I17" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K17" s="32">
         <v>0</v>
@@ -7009,25 +7009,25 @@
         <v>28</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="71" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I18" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K18" s="32">
         <v>0</v>
@@ -7047,25 +7047,25 @@
         <v>54</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="71" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I19" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K19" s="32">
         <v>0</v>
@@ -7082,28 +7082,28 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="70" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G20" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H20" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I20" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K20" s="32">
         <v>0</v>
@@ -7120,28 +7120,28 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="70" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B21" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I21" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K21" s="32">
         <v>0</v>
@@ -7158,28 +7158,28 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B22" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C22" s="77" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I22" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K22" s="32">
         <v>0</v>
@@ -7196,28 +7196,28 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="70" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I23" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K23" s="32">
         <v>0</v>
@@ -7234,15 +7234,15 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F24" s="80" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="90" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
+      <c r="A27" s="97" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
       <c r="F27" s="79" t="s">
         <v>7</v>
       </c>
@@ -7256,10 +7256,10 @@
         <v>12</v>
       </c>
       <c r="J27" s="79" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K27" s="79" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -7273,7 +7273,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>39</v>
@@ -7282,7 +7282,7 @@
         <v>39</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J28" s="8">
         <v>0</v>
@@ -7296,13 +7296,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>18</v>
@@ -7311,7 +7311,7 @@
         <v>24</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J29" s="8">
         <v>1</v>
@@ -7325,22 +7325,22 @@
         <v>8</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="83" t="s">
         <v>23</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J30" s="8">
         <v>1</v>
@@ -7354,22 +7354,22 @@
         <v>9</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="83" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J31" s="8">
         <v>1</v>
@@ -7383,22 +7383,22 @@
         <v>12</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="83" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J32" s="8">
         <v>1</v>
@@ -7409,25 +7409,25 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="84" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B33" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J33" s="8">
         <v>1</v>
@@ -7438,21 +7438,21 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="84" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B34" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="78" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F34" s="74" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F35" s="74" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -7469,6 +7469,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F33A6DB98216B5448738561EEB5E52F3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b9409f311f3f1f262294d1b1bffdd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2cc8eddb-c4fa-487b-b5b5-3b55fe26257b" xmlns:ns3="d3a4b13c-8f4e-44e8-9732-bc540be98408" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bff76ea5e37bf585a119dc8c50450aee" ns2:_="" ns3:_="">
     <xsd:import namespace="2cc8eddb-c4fa-487b-b5b5-3b55fe26257b"/>
@@ -7679,22 +7694,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CC594F-C037-4148-B9F5-575D82E062CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE803B83-899C-4D1E-8DBC-13369AC549E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6DE800C-9F6D-468E-B968-BE9FB6D7D6B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7711,21 +7728,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE803B83-899C-4D1E-8DBC-13369AC549E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CC594F-C037-4148-B9F5-575D82E062CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>